<commit_message>
Put buglist on gitignore list
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Prio [1-3]</t>
+  </si>
+  <si>
+    <t>Idee zur besseren Umsetzung im Code, aber kein Bug</t>
+  </si>
+  <si>
+    <t>TrainingScheduleOverview-Diagramm wird mit Element, dass die category null hat, für "Gesamt" gebaut. Das fühlt sich nach einem Hack an. Vllt kann man das noch mal überprüfen. Vllt kann man das Übergeben einer Category im Konstruktor auch rausnehmen?</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <dimension ref="B2:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,8 +469,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+    <row r="4" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="E4" s="1"/>
       <c r="H4">
@@ -489,6 +497,12 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="1"/>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>

</xml_diff>